<commit_message>
Reading data by aggregate function
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BA course materials\R programs\R-Project1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Additional Qualifications\R programs\R-Project01\R-Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="16">
   <si>
     <t>rollno</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>J</t>
+  </si>
+  <si>
+    <t>salary</t>
   </si>
 </sst>
 </file>
@@ -556,15 +559,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -577,8 +580,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10</v>
       </c>
@@ -591,8 +597,11 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>11</v>
       </c>
@@ -605,8 +614,11 @@
       <c r="D3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>12</v>
       </c>
@@ -619,8 +631,11 @@
       <c r="D4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>13</v>
       </c>
@@ -633,8 +648,11 @@
       <c r="D5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>14</v>
       </c>
@@ -647,8 +665,11 @@
       <c r="D6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>15</v>
       </c>
@@ -661,8 +682,11 @@
       <c r="D7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>16</v>
       </c>
@@ -675,8 +699,11 @@
       <c r="D8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>17</v>
       </c>
@@ -689,8 +716,11 @@
       <c r="D9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>18</v>
       </c>
@@ -703,8 +733,11 @@
       <c r="D10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>19</v>
       </c>
@@ -716,6 +749,9 @@
       </c>
       <c r="D11" t="s">
         <v>5</v>
+      </c>
+      <c r="E11">
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>